<commit_message>
add upload to tracker as well
</commit_message>
<xml_diff>
--- a/tracker/config_error_tracker.xlsx
+++ b/tracker/config_error_tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="113">
   <si>
     <t>BUSINESS_UNIT</t>
   </si>
@@ -67,6 +67,9 @@
     <t>SRGBU</t>
   </si>
   <si>
+    <t>EBBU</t>
+  </si>
+  <si>
     <t>C9400</t>
   </si>
   <si>
@@ -205,6 +208,21 @@
     <t>111979248-3</t>
   </si>
   <si>
+    <t>111911578-1</t>
+  </si>
+  <si>
+    <t>111911578-3</t>
+  </si>
+  <si>
+    <t>111921642-10</t>
+  </si>
+  <si>
+    <t>112079091-4</t>
+  </si>
+  <si>
+    <t>112079091-7</t>
+  </si>
+  <si>
     <t>C9410R</t>
   </si>
   <si>
@@ -232,6 +250,12 @@
     <t>ISR1100X-4G</t>
   </si>
   <si>
+    <t>C9500-16X-A</t>
+  </si>
+  <si>
+    <t>C1100TG-1N32A</t>
+  </si>
+  <si>
     <t>09/18/2020</t>
   </si>
   <si>
@@ -320,6 +344,15 @@
   </si>
   <si>
     <t>Missing PSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(user report) Missing power supply or power supply blank, please add 2 units PWR-C4-BLANK </t>
+  </si>
+  <si>
+    <t>(user report) NIM-ES2-8, NIM-LTEA-EA need remove one of them</t>
+  </si>
+  <si>
+    <t>(user report) NIM-ES2-8 duplicated, need remove one</t>
   </si>
 </sst>
 </file>
@@ -327,7 +360,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -681,7 +714,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -730,25 +763,25 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K2" s="2">
         <v>44249</v>
@@ -762,25 +795,25 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K3" s="2">
         <v>44249</v>
@@ -794,25 +827,25 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K4" s="2">
         <v>44249</v>
@@ -826,25 +859,25 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K5" s="2">
         <v>44249</v>
@@ -858,25 +891,25 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K6" s="2">
         <v>44249</v>
@@ -890,25 +923,25 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K7" s="2">
         <v>44249</v>
@@ -922,25 +955,25 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K8" s="2">
         <v>44249</v>
@@ -954,25 +987,25 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K9" s="2">
         <v>44249</v>
@@ -986,25 +1019,25 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K10" s="2">
         <v>44249</v>
@@ -1018,25 +1051,25 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J11" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K11" s="2">
         <v>44249</v>
@@ -1050,25 +1083,25 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K12" s="2">
         <v>44249</v>
@@ -1082,28 +1115,28 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I13" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="J13" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K13" s="2">
         <v>44249</v>
@@ -1117,28 +1150,28 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="J14" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="K14" s="2">
         <v>44249</v>
@@ -1152,25 +1185,25 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K15" s="2">
         <v>44249</v>
@@ -1184,25 +1217,25 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="J16" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K16" s="2">
         <v>44249</v>
@@ -1216,25 +1249,25 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="J17" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K17" s="2">
         <v>44249</v>
@@ -1248,25 +1281,25 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J18" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="K18" s="2">
         <v>44249</v>
@@ -1280,28 +1313,28 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I19" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J19" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K19" s="2">
         <v>44249</v>
@@ -1315,28 +1348,28 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J20" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K20" s="2">
         <v>44249</v>
@@ -1350,28 +1383,28 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I21" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J21" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K21" s="2">
         <v>44249</v>
@@ -1385,28 +1418,28 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I22" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J22" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K22" s="2">
         <v>44249</v>
@@ -1420,28 +1453,28 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I23" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J23" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K23" s="2">
         <v>44249</v>
@@ -1455,28 +1488,28 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="I24" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J24" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K24" s="2">
         <v>44249</v>
@@ -1490,28 +1523,28 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I25" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J25" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K25" s="2">
         <v>44249</v>
@@ -1525,28 +1558,28 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J26" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K26" s="2">
         <v>44249</v>
@@ -1560,28 +1593,28 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I27" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J27" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K27" s="2">
         <v>44249</v>
@@ -1595,28 +1628,28 @@
         <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I28" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J28" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K28" s="2">
         <v>44249</v>
@@ -1630,28 +1663,28 @@
         <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I29" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J29" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K29" s="2">
         <v>44249</v>
@@ -1665,28 +1698,28 @@
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I30" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J30" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K30" s="2">
         <v>44249</v>
@@ -1700,28 +1733,28 @@
         <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J31" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K31" s="2">
         <v>44249</v>
@@ -1735,28 +1768,28 @@
         <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="I32" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J32" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K32" s="2">
         <v>44249</v>
@@ -1770,28 +1803,28 @@
         <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I33" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J33" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K33" s="2">
         <v>44249</v>
@@ -1805,28 +1838,28 @@
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="I34" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J34" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K34" s="2">
         <v>44249</v>
@@ -1840,28 +1873,28 @@
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="I35" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="J35" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="K35" s="2">
         <v>44249</v>
@@ -1875,28 +1908,28 @@
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="I36" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="J36" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="K36" s="2">
         <v>44249</v>
@@ -1910,25 +1943,25 @@
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="J37" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K37" s="2">
         <v>44250</v>
@@ -1942,25 +1975,25 @@
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="J38" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K38" s="2">
         <v>44250</v>
@@ -1974,25 +2007,25 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="J39" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K39" s="2">
         <v>44250</v>
@@ -2006,25 +2039,25 @@
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="J40" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K40" s="2">
         <v>44250</v>
@@ -2038,25 +2071,25 @@
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="J41" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K41" s="2">
         <v>44250</v>
@@ -2070,25 +2103,25 @@
         <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="J42" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="K42" s="2">
         <v>44250</v>
@@ -2102,31 +2135,161 @@
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="I43" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="J43" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="K43" s="2">
         <v>44251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="J44" t="s">
+        <v>110</v>
+      </c>
+      <c r="K44" s="2">
+        <v>44278.67979943893</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="J45" t="s">
+        <v>110</v>
+      </c>
+      <c r="K45" s="2">
+        <v>44278.67979943893</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="J46" t="s">
+        <v>111</v>
+      </c>
+      <c r="K46" s="2">
+        <v>44278.67979943893</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>112</v>
+      </c>
+      <c r="K47" s="2">
+        <v>44278.67979943893</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>112</v>
+      </c>
+      <c r="K48" s="2">
+        <v>44278.67979943893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change tracker to db
</commit_message>
<xml_diff>
--- a/tracker/config_error_tracker.xlsx
+++ b/tracker/config_error_tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>BUSINESS_UNIT</t>
   </si>
@@ -61,13 +61,67 @@
     <t>111931089-2</t>
   </si>
   <si>
+    <t>111142195-37</t>
+  </si>
+  <si>
+    <t>111142195-41</t>
+  </si>
+  <si>
+    <t>111142195-47</t>
+  </si>
+  <si>
+    <t>111142918-4</t>
+  </si>
+  <si>
+    <t>111142195-54</t>
+  </si>
+  <si>
+    <t>111142195-59</t>
+  </si>
+  <si>
+    <t>111142195-73</t>
+  </si>
+  <si>
+    <t>111142195-77</t>
+  </si>
+  <si>
+    <t>111142195-81</t>
+  </si>
+  <si>
+    <t>111142195-85</t>
+  </si>
+  <si>
+    <t>111142195-89</t>
+  </si>
+  <si>
+    <t>111424230-2</t>
+  </si>
+  <si>
+    <t>111401757-3</t>
+  </si>
+  <si>
+    <t>112466942-1</t>
+  </si>
+  <si>
     <t>C9410R-96U-BNDL-A</t>
   </si>
   <si>
+    <t>C9410R</t>
+  </si>
+  <si>
+    <t>C9407R-96U-BNDL-A</t>
+  </si>
+  <si>
+    <t>ISR4331-DNA</t>
+  </si>
+  <si>
     <t>02/11/2021</t>
   </si>
   <si>
     <t>SUP qty over</t>
+  </si>
+  <si>
+    <t>(user report) test</t>
   </si>
 </sst>
 </file>
@@ -429,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -487,19 +541,383 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="K2" s="2">
         <v>44249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="2">
+        <v>44348.42330030093</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="2">
+        <v>44348.42637737964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>